<commit_message>
[perf]: optimización codigo. * codigo limpio y más legible, - se agrega un codigo css que me permite personalizar las vistas form del sitio web. - se renombran archivos, campos, se mejora la estructura del modulo en general.
</commit_message>
<xml_diff>
--- a/static/download/plantilla_ejemplo.xlsx
+++ b/static/download/plantilla_ejemplo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBASTIAN\Documents\Mis proyectos\Odoo\Prueba tecnica - Votaciones - Odoov16\odoo\addons_personalizados\ges_votaciones\static\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBASTIAN\Documents\Mis proyectos\Odoo\Prueba tecnica - Votaciones - Odoov16\odoo\addons_personalizados\ges_votaciones\static\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EC9CAF-F25D-4E8E-86E5-921E26882F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D984B67B-2C05-421A-872B-3A86565B0B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Descripcion</t>
   </si>
@@ -31,16 +31,31 @@
     <t>Fecha_inicio</t>
   </si>
   <si>
-    <t>Ejemplo nombre proceso de votación x</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Sede Chile</t>
-  </si>
-  <si>
     <t>Nombre_sede</t>
+  </si>
+  <si>
+    <t>Sede Colombia</t>
+  </si>
+  <si>
+    <t>Sede Bélgica</t>
+  </si>
+  <si>
+    <t>Sede Argentina</t>
+  </si>
+  <si>
+    <t>Sede Venezuela</t>
+  </si>
+  <si>
+    <t>Proceso Ejemplo sede U colombia</t>
+  </si>
+  <si>
+    <t>Proceso Ejemplo sede U argentina</t>
+  </si>
+  <si>
+    <t>Proceso Ejemplo sede U venezuela</t>
+  </si>
+  <si>
+    <t>Proceso Ejemplo sede U bélgica</t>
   </si>
 </sst>
 </file>
@@ -431,22 +446,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="5" width="30.6640625" customWidth="1"/>
+    <col min="3" max="4" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -457,24 +472,62 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3">
-        <v>45110</v>
+        <v>45108</v>
       </c>
       <c r="D2" s="3">
         <v>45117</v>
       </c>
-      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45109</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45110</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45111</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>